<commit_message>
Added no color run
</commit_message>
<xml_diff>
--- a/compare 15 with 10 augmentations.xlsx
+++ b/compare 15 with 10 augmentations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chris/dev/uni/vision/AISSCV_results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94B446FF-47FB-784F-BC80-1CE664D19913}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13EADBC3-4877-C145-9CB7-E66A0F66B4D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26920" yWindow="500" windowWidth="60160" windowHeight="32080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30080" yWindow="500" windowWidth="30080" windowHeight="32080" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="42">
   <si>
     <t>run</t>
   </si>
@@ -152,6 +152,12 @@
   </si>
   <si>
     <t>FP Difference</t>
+  </si>
+  <si>
+    <t>No Color</t>
+  </si>
+  <si>
+    <t>Color</t>
   </si>
 </sst>
 </file>
@@ -159,9 +165,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.000%"/>
+    <numFmt numFmtId="164" formatCode="0.000%"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -173,6 +179,7 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -203,6 +210,14 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -212,7 +227,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -239,6 +254,162 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
       <bottom style="double">
         <color indexed="64"/>
       </bottom>
@@ -246,7 +417,9 @@
     </border>
     <border>
       <left/>
-      <right/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
       <top/>
       <bottom style="thin">
         <color auto="1"/>
@@ -261,71 +434,8 @@
       <top style="thin">
         <color auto="1"/>
       </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thick">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thick">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thick">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
+      <bottom style="double">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -334,28 +444,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -363,11 +461,15 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -375,16 +477,136 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Per cent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="12">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -726,39 +948,39 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:T8"/>
+  <dimension ref="A1:T17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:20" ht="58" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="9" t="s">
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="9"/>
-      <c r="O1" s="9"/>
-      <c r="P1" s="9"/>
-      <c r="Q1" s="9"/>
-      <c r="R1" s="9"/>
-      <c r="S1" s="9"/>
-      <c r="T1" s="9"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
+      <c r="N1" s="10"/>
+      <c r="O1" s="10"/>
+      <c r="P1" s="10"/>
+      <c r="Q1" s="10"/>
+      <c r="R1" s="10"/>
+      <c r="S1" s="10"/>
+      <c r="T1" s="10"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -788,13 +1010,13 @@
       <c r="I2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="J2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="K2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="L2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="M2" s="1" t="s">
@@ -826,61 +1048,61 @@
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="14">
+      <c r="B3" s="8">
         <v>0.25</v>
       </c>
-      <c r="C3" s="14">
+      <c r="C3" s="8">
         <v>0.78</v>
       </c>
-      <c r="D3" s="14">
+      <c r="D3" s="8">
         <v>0.82</v>
       </c>
-      <c r="E3" s="14">
+      <c r="E3" s="8">
         <v>0.8</v>
       </c>
-      <c r="F3" s="14">
+      <c r="F3" s="8">
         <v>212</v>
       </c>
-      <c r="G3" s="14">
+      <c r="G3" s="8">
         <v>60</v>
       </c>
-      <c r="H3" s="14">
+      <c r="H3" s="8">
         <v>48</v>
       </c>
-      <c r="I3" s="14">
+      <c r="I3" s="8">
         <v>0.59340000000000004</v>
       </c>
-      <c r="J3" s="19">
+      <c r="J3" s="9">
         <v>0.881992</v>
       </c>
-      <c r="K3" s="5" t="s">
+      <c r="K3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L3">
+      <c r="L3" s="8">
         <v>0.25</v>
       </c>
-      <c r="M3">
+      <c r="M3" s="8">
         <v>0.8</v>
       </c>
-      <c r="N3">
+      <c r="N3" s="8">
         <v>0.83</v>
       </c>
-      <c r="O3">
+      <c r="O3" s="8">
         <v>0.82</v>
       </c>
-      <c r="P3" s="3">
+      <c r="P3" s="21">
         <v>216</v>
       </c>
-      <c r="Q3" s="3">
+      <c r="Q3" s="21">
         <v>54</v>
       </c>
-      <c r="R3" s="3">
+      <c r="R3" s="21">
         <v>44</v>
       </c>
-      <c r="S3">
+      <c r="S3" s="8">
         <v>0.60860000000000003</v>
       </c>
-      <c r="T3">
+      <c r="T3" s="8">
         <v>0.87446999999999997</v>
       </c>
     </row>
@@ -888,61 +1110,61 @@
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="14">
+      <c r="B4" s="8">
         <v>0.25</v>
       </c>
-      <c r="C4" s="14">
+      <c r="C4" s="8">
         <v>0.8</v>
       </c>
-      <c r="D4" s="14">
+      <c r="D4" s="8">
         <v>0.81</v>
       </c>
-      <c r="E4" s="14">
+      <c r="E4" s="8">
         <v>0.8</v>
       </c>
-      <c r="F4" s="14">
+      <c r="F4" s="8">
         <v>212</v>
       </c>
-      <c r="G4" s="14">
+      <c r="G4" s="8">
         <v>53</v>
       </c>
-      <c r="H4" s="14">
+      <c r="H4" s="8">
         <v>51</v>
       </c>
-      <c r="I4" s="14">
+      <c r="I4" s="8">
         <v>0.60099999999999998</v>
       </c>
-      <c r="J4" s="19">
+      <c r="J4" s="9">
         <v>0.88091900000000001</v>
       </c>
-      <c r="K4" s="5" t="s">
+      <c r="K4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="L4">
+      <c r="L4" s="8">
         <v>0.25</v>
       </c>
-      <c r="M4">
+      <c r="M4" s="8">
         <v>0.78</v>
       </c>
-      <c r="N4">
+      <c r="N4" s="8">
         <v>0.79</v>
       </c>
-      <c r="O4">
+      <c r="O4" s="8">
         <v>0.79</v>
       </c>
-      <c r="P4" s="3">
+      <c r="P4" s="21">
         <v>209</v>
       </c>
-      <c r="Q4" s="3">
+      <c r="Q4" s="21">
         <v>58</v>
       </c>
-      <c r="R4" s="3">
+      <c r="R4" s="21">
         <v>54</v>
       </c>
-      <c r="S4">
+      <c r="S4" s="8">
         <v>0.59050000000000002</v>
       </c>
-      <c r="T4">
+      <c r="T4" s="8">
         <v>0.89104799999999995</v>
       </c>
     </row>
@@ -950,61 +1172,61 @@
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="14">
+      <c r="B5" s="8">
         <v>0.25</v>
       </c>
-      <c r="C5" s="14">
+      <c r="C5" s="8">
         <v>0.8</v>
       </c>
-      <c r="D5" s="14">
+      <c r="D5" s="8">
         <v>0.82</v>
       </c>
-      <c r="E5" s="14">
+      <c r="E5" s="8">
         <v>0.81</v>
       </c>
-      <c r="F5" s="14">
+      <c r="F5" s="8">
         <v>216</v>
       </c>
-      <c r="G5" s="14">
+      <c r="G5" s="8">
         <v>54</v>
       </c>
-      <c r="H5" s="14">
+      <c r="H5" s="8">
         <v>48</v>
       </c>
-      <c r="I5" s="14">
+      <c r="I5" s="8">
         <v>0.60189999999999999</v>
       </c>
-      <c r="J5" s="19">
+      <c r="J5" s="9">
         <v>0.87656500000000004</v>
       </c>
-      <c r="K5" s="5" t="s">
+      <c r="K5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="L5">
+      <c r="L5" s="8">
         <v>0.25</v>
       </c>
-      <c r="M5">
+      <c r="M5" s="8">
         <v>0.84</v>
       </c>
-      <c r="N5">
+      <c r="N5" s="8">
         <v>0.83</v>
       </c>
-      <c r="O5">
+      <c r="O5" s="8">
         <v>0.84</v>
       </c>
-      <c r="P5" s="3">
+      <c r="P5" s="21">
         <v>218</v>
       </c>
-      <c r="Q5" s="3">
+      <c r="Q5" s="21">
         <v>40</v>
       </c>
-      <c r="R5" s="3">
+      <c r="R5" s="21">
         <v>46</v>
       </c>
-      <c r="S5">
+      <c r="S5" s="8">
         <v>0.64100000000000001</v>
       </c>
-      <c r="T5">
+      <c r="T5" s="8">
         <v>0.881189</v>
       </c>
     </row>
@@ -1012,210 +1234,690 @@
       <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="14">
+      <c r="B6" s="8">
         <v>0.25</v>
       </c>
-      <c r="C6" s="14">
+      <c r="C6" s="8">
         <v>0.83</v>
       </c>
-      <c r="D6" s="14">
+      <c r="D6" s="8">
         <v>0.82</v>
       </c>
-      <c r="E6" s="14">
+      <c r="E6" s="8">
         <v>0.83</v>
       </c>
-      <c r="F6" s="14">
+      <c r="F6" s="8">
         <v>221</v>
       </c>
-      <c r="G6" s="14">
+      <c r="G6" s="8">
         <v>46</v>
       </c>
-      <c r="H6" s="14">
+      <c r="H6" s="8">
         <v>47</v>
       </c>
-      <c r="I6" s="14">
+      <c r="I6" s="8">
         <v>0.62929999999999997</v>
       </c>
-      <c r="J6" s="19">
+      <c r="J6" s="9">
         <v>0.88683500000000004</v>
       </c>
-      <c r="K6" s="5" t="s">
+      <c r="K6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="L6">
+      <c r="L6" s="8">
         <v>0.25</v>
       </c>
-      <c r="M6">
+      <c r="M6" s="8">
         <v>0.78</v>
       </c>
-      <c r="N6">
+      <c r="N6" s="8">
         <v>0.8</v>
       </c>
-      <c r="O6">
+      <c r="O6" s="8">
         <v>0.79</v>
       </c>
-      <c r="P6" s="3">
+      <c r="P6" s="21">
         <v>215</v>
       </c>
-      <c r="Q6" s="3">
+      <c r="Q6" s="21">
         <v>61</v>
       </c>
-      <c r="R6" s="3">
+      <c r="R6" s="21">
         <v>53</v>
       </c>
-      <c r="S6">
+      <c r="S6" s="8">
         <v>0.59130000000000005</v>
       </c>
-      <c r="T6">
+      <c r="T6" s="8">
         <v>0.87364200000000003</v>
       </c>
     </row>
     <row r="7" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="14">
+      <c r="B7" s="26">
         <v>0.25</v>
       </c>
-      <c r="C7" s="14">
+      <c r="C7" s="26">
         <v>0.78</v>
       </c>
-      <c r="D7" s="14">
+      <c r="D7" s="26">
         <v>0.77</v>
       </c>
-      <c r="E7" s="14">
+      <c r="E7" s="26">
         <v>0.78</v>
       </c>
-      <c r="F7" s="14">
+      <c r="F7" s="26">
         <v>200</v>
       </c>
-      <c r="G7" s="14">
+      <c r="G7" s="26">
         <v>57</v>
       </c>
-      <c r="H7" s="14">
+      <c r="H7" s="26">
         <v>59</v>
       </c>
-      <c r="I7" s="14">
+      <c r="I7" s="26">
         <v>0.59689999999999999</v>
       </c>
-      <c r="J7" s="19">
+      <c r="J7" s="27">
         <v>0.85829699999999998</v>
       </c>
-      <c r="K7" s="5" t="s">
+      <c r="K7" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="L7" s="2">
+      <c r="L7" s="26">
         <v>0.25</v>
       </c>
-      <c r="M7" s="2">
+      <c r="M7" s="26">
         <v>0.77</v>
       </c>
-      <c r="N7" s="2">
+      <c r="N7" s="26">
         <v>0.8</v>
       </c>
-      <c r="O7" s="2">
+      <c r="O7" s="26">
         <v>0.78</v>
       </c>
-      <c r="P7" s="4">
+      <c r="P7" s="30">
         <v>208</v>
       </c>
-      <c r="Q7" s="4">
+      <c r="Q7" s="30">
         <v>63</v>
       </c>
-      <c r="R7" s="4">
+      <c r="R7" s="30">
         <v>51</v>
       </c>
-      <c r="S7" s="2">
+      <c r="S7" s="26">
         <v>0.5887</v>
       </c>
-      <c r="T7" s="2">
+      <c r="T7" s="26">
         <v>0.86971500000000002</v>
       </c>
     </row>
     <row r="8" spans="1:20" ht="16" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="14">
+      <c r="B8" s="31">
         <f>MEDIAN(B3:B7)</f>
         <v>0.25</v>
       </c>
-      <c r="C8" s="14">
+      <c r="C8" s="31">
         <f t="shared" ref="C8:J8" si="0">MEDIAN(C3:C7)</f>
         <v>0.8</v>
       </c>
-      <c r="D8" s="14">
+      <c r="D8" s="31">
         <f t="shared" si="0"/>
         <v>0.82</v>
       </c>
-      <c r="E8" s="14">
+      <c r="E8" s="31">
         <f t="shared" si="0"/>
         <v>0.8</v>
       </c>
-      <c r="F8" s="14">
+      <c r="F8" s="31">
         <f t="shared" si="0"/>
         <v>212</v>
       </c>
-      <c r="G8" s="14">
+      <c r="G8" s="31">
         <f t="shared" si="0"/>
         <v>54</v>
       </c>
-      <c r="H8" s="14">
+      <c r="H8" s="31">
         <f t="shared" si="0"/>
         <v>48</v>
       </c>
-      <c r="I8" s="14">
+      <c r="I8" s="31">
         <f t="shared" si="0"/>
         <v>0.60099999999999998</v>
       </c>
-      <c r="J8" s="19">
+      <c r="J8" s="33">
         <f t="shared" si="0"/>
         <v>0.88091900000000001</v>
       </c>
-      <c r="K8" s="5" t="s">
+      <c r="K8" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="L8">
+      <c r="L8" s="31">
         <f>MEDIAN(L3:L7)</f>
         <v>0.25</v>
       </c>
-      <c r="M8">
+      <c r="M8" s="31">
         <f t="shared" ref="M8:T8" si="1">MEDIAN(M3:M7)</f>
         <v>0.78</v>
       </c>
-      <c r="N8">
+      <c r="N8" s="31">
         <f t="shared" si="1"/>
         <v>0.8</v>
       </c>
-      <c r="O8">
+      <c r="O8" s="31">
         <f t="shared" si="1"/>
         <v>0.79</v>
       </c>
-      <c r="P8">
+      <c r="P8" s="31">
         <f t="shared" si="1"/>
         <v>215</v>
       </c>
-      <c r="Q8">
+      <c r="Q8" s="31">
         <f t="shared" si="1"/>
         <v>58</v>
       </c>
-      <c r="R8">
+      <c r="R8" s="31">
         <f t="shared" si="1"/>
         <v>51</v>
       </c>
-      <c r="S8">
+      <c r="S8" s="31">
         <f t="shared" si="1"/>
         <v>0.59130000000000005</v>
       </c>
-      <c r="T8">
+      <c r="T8" s="31">
         <f t="shared" si="1"/>
         <v>0.87446999999999997</v>
       </c>
     </row>
+    <row r="10" spans="1:20" ht="29" x14ac:dyDescent="0.2">
+      <c r="A10" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="L10" s="34"/>
+      <c r="M10" s="34"/>
+      <c r="N10" s="34"/>
+      <c r="O10" s="34"/>
+      <c r="P10" s="34"/>
+      <c r="Q10" s="34"/>
+      <c r="R10" s="34"/>
+      <c r="S10" s="34"/>
+      <c r="T10" s="34"/>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="O11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="R11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="S11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="T11" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="8">
+        <v>0.25</v>
+      </c>
+      <c r="C12" s="8">
+        <v>0.59</v>
+      </c>
+      <c r="D12" s="8">
+        <v>0.39</v>
+      </c>
+      <c r="E12" s="8">
+        <v>0.47</v>
+      </c>
+      <c r="F12" s="8">
+        <v>102</v>
+      </c>
+      <c r="G12" s="8">
+        <v>71</v>
+      </c>
+      <c r="H12" s="8">
+        <v>158</v>
+      </c>
+      <c r="I12" s="8">
+        <v>0.39779999999999999</v>
+      </c>
+      <c r="J12" s="9">
+        <v>0.58740099999999995</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L12" s="8">
+        <v>0.25</v>
+      </c>
+      <c r="M12" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="N12" s="8">
+        <v>0.83</v>
+      </c>
+      <c r="O12" s="8">
+        <v>0.82</v>
+      </c>
+      <c r="P12" s="21">
+        <v>216</v>
+      </c>
+      <c r="Q12" s="21">
+        <v>54</v>
+      </c>
+      <c r="R12" s="21">
+        <v>44</v>
+      </c>
+      <c r="S12" s="8">
+        <v>0.60860000000000003</v>
+      </c>
+      <c r="T12" s="8">
+        <v>0.87446999999999997</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="8">
+        <v>0.25</v>
+      </c>
+      <c r="C13" s="8">
+        <v>0.69</v>
+      </c>
+      <c r="D13" s="8">
+        <v>0.45</v>
+      </c>
+      <c r="E13" s="8">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="F13" s="8">
+        <v>119</v>
+      </c>
+      <c r="G13" s="8">
+        <v>53</v>
+      </c>
+      <c r="H13" s="8">
+        <v>144</v>
+      </c>
+      <c r="I13" s="8">
+        <v>0.47589999999999999</v>
+      </c>
+      <c r="J13" s="9">
+        <v>0.648254</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L13" s="8">
+        <v>0.25</v>
+      </c>
+      <c r="M13" s="8">
+        <v>0.78</v>
+      </c>
+      <c r="N13" s="8">
+        <v>0.79</v>
+      </c>
+      <c r="O13" s="8">
+        <v>0.79</v>
+      </c>
+      <c r="P13" s="21">
+        <v>209</v>
+      </c>
+      <c r="Q13" s="21">
+        <v>58</v>
+      </c>
+      <c r="R13" s="21">
+        <v>54</v>
+      </c>
+      <c r="S13" s="8">
+        <v>0.59050000000000002</v>
+      </c>
+      <c r="T13" s="8">
+        <v>0.89104799999999995</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="8">
+        <v>0.25</v>
+      </c>
+      <c r="C14" s="8">
+        <v>0.61</v>
+      </c>
+      <c r="D14" s="8">
+        <v>0.42</v>
+      </c>
+      <c r="E14" s="8">
+        <v>0.49</v>
+      </c>
+      <c r="F14" s="8">
+        <v>110</v>
+      </c>
+      <c r="G14" s="8">
+        <v>71</v>
+      </c>
+      <c r="H14" s="8">
+        <v>154</v>
+      </c>
+      <c r="I14" s="8">
+        <v>0.42070000000000002</v>
+      </c>
+      <c r="J14" s="9">
+        <v>0.60589800000000005</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L14" s="8">
+        <v>0.25</v>
+      </c>
+      <c r="M14" s="8">
+        <v>0.84</v>
+      </c>
+      <c r="N14" s="8">
+        <v>0.83</v>
+      </c>
+      <c r="O14" s="8">
+        <v>0.84</v>
+      </c>
+      <c r="P14" s="21">
+        <v>218</v>
+      </c>
+      <c r="Q14" s="21">
+        <v>40</v>
+      </c>
+      <c r="R14" s="21">
+        <v>46</v>
+      </c>
+      <c r="S14" s="8">
+        <v>0.64100000000000001</v>
+      </c>
+      <c r="T14" s="8">
+        <v>0.881189</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="8">
+        <v>0.25</v>
+      </c>
+      <c r="C15" s="8">
+        <v>0.69</v>
+      </c>
+      <c r="D15" s="8">
+        <v>0.42</v>
+      </c>
+      <c r="E15" s="8">
+        <v>0.52</v>
+      </c>
+      <c r="F15" s="8">
+        <v>112</v>
+      </c>
+      <c r="G15" s="8">
+        <v>51</v>
+      </c>
+      <c r="H15" s="8">
+        <v>156</v>
+      </c>
+      <c r="I15" s="8">
+        <v>0.48130000000000001</v>
+      </c>
+      <c r="J15" s="9">
+        <v>0.65812999999999999</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="L15" s="8">
+        <v>0.25</v>
+      </c>
+      <c r="M15" s="8">
+        <v>0.78</v>
+      </c>
+      <c r="N15" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="O15" s="8">
+        <v>0.79</v>
+      </c>
+      <c r="P15" s="21">
+        <v>215</v>
+      </c>
+      <c r="Q15" s="21">
+        <v>61</v>
+      </c>
+      <c r="R15" s="21">
+        <v>53</v>
+      </c>
+      <c r="S15" s="8">
+        <v>0.59130000000000005</v>
+      </c>
+      <c r="T15" s="8">
+        <v>0.87364200000000003</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="26">
+        <v>0.25</v>
+      </c>
+      <c r="C16" s="26">
+        <v>0.6</v>
+      </c>
+      <c r="D16" s="26">
+        <v>0.42</v>
+      </c>
+      <c r="E16" s="26">
+        <v>0.5</v>
+      </c>
+      <c r="F16" s="26">
+        <v>110</v>
+      </c>
+      <c r="G16" s="26">
+        <v>72</v>
+      </c>
+      <c r="H16" s="26">
+        <v>149</v>
+      </c>
+      <c r="I16" s="26">
+        <v>0.41539999999999999</v>
+      </c>
+      <c r="J16" s="27">
+        <v>0.60148800000000002</v>
+      </c>
+      <c r="K16" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="L16" s="26">
+        <v>0.25</v>
+      </c>
+      <c r="M16" s="26">
+        <v>0.77</v>
+      </c>
+      <c r="N16" s="26">
+        <v>0.8</v>
+      </c>
+      <c r="O16" s="26">
+        <v>0.78</v>
+      </c>
+      <c r="P16" s="30">
+        <v>208</v>
+      </c>
+      <c r="Q16" s="30">
+        <v>63</v>
+      </c>
+      <c r="R16" s="30">
+        <v>51</v>
+      </c>
+      <c r="S16" s="26">
+        <v>0.5887</v>
+      </c>
+      <c r="T16" s="26">
+        <v>0.86971500000000002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="23">
+        <f>MEDIAN(B12:B16)</f>
+        <v>0.25</v>
+      </c>
+      <c r="C17" s="23">
+        <f t="shared" ref="C17:J17" si="2">MEDIAN(C12:C16)</f>
+        <v>0.61</v>
+      </c>
+      <c r="D17" s="23">
+        <f t="shared" si="2"/>
+        <v>0.42</v>
+      </c>
+      <c r="E17" s="23">
+        <f t="shared" si="2"/>
+        <v>0.5</v>
+      </c>
+      <c r="F17" s="23">
+        <f t="shared" si="2"/>
+        <v>110</v>
+      </c>
+      <c r="G17" s="23">
+        <f t="shared" si="2"/>
+        <v>71</v>
+      </c>
+      <c r="H17" s="23">
+        <f t="shared" si="2"/>
+        <v>154</v>
+      </c>
+      <c r="I17" s="23">
+        <f t="shared" si="2"/>
+        <v>0.42070000000000002</v>
+      </c>
+      <c r="J17" s="24">
+        <f t="shared" si="2"/>
+        <v>0.60589800000000005</v>
+      </c>
+      <c r="K17" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="L17" s="23">
+        <f>MEDIAN(L12:L16)</f>
+        <v>0.25</v>
+      </c>
+      <c r="M17" s="23">
+        <f t="shared" ref="M17:T17" si="3">MEDIAN(M12:M16)</f>
+        <v>0.78</v>
+      </c>
+      <c r="N17" s="23">
+        <f t="shared" si="3"/>
+        <v>0.8</v>
+      </c>
+      <c r="O17" s="23">
+        <f t="shared" si="3"/>
+        <v>0.79</v>
+      </c>
+      <c r="P17" s="23">
+        <f t="shared" si="3"/>
+        <v>215</v>
+      </c>
+      <c r="Q17" s="23">
+        <f t="shared" si="3"/>
+        <v>58</v>
+      </c>
+      <c r="R17" s="23">
+        <f t="shared" si="3"/>
+        <v>51</v>
+      </c>
+      <c r="S17" s="23">
+        <f t="shared" si="3"/>
+        <v>0.59130000000000005</v>
+      </c>
+      <c r="T17" s="23">
+        <f t="shared" si="3"/>
+        <v>0.87446999999999997</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="K1:T1"/>
     <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A10:J10"/>
+    <mergeCell ref="K10:T10"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" scale="69" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
@@ -1227,10 +1929,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L16"/>
+  <dimension ref="A1:L34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1241,71 +1943,71 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="7" t="s">
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="H2" s="10" t="s">
+      <c r="H2" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="J2" s="11" t="s">
+      <c r="J2" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="K2" s="11" t="s">
+      <c r="K2" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="L2" s="11" t="s">
+      <c r="L2" s="5" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="12">
+      <c r="B3" s="18">
         <v>0.92427999999999988</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="19">
         <v>13.8</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="20">
         <v>5</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="12">
+      <c r="F3" s="6">
         <v>0.92495999999999989</v>
       </c>
       <c r="G3">
@@ -1314,7 +2016,7 @@
       <c r="H3">
         <v>4.5999999999999996</v>
       </c>
-      <c r="J3" s="13">
+      <c r="J3" s="7">
         <f>B3-F3</f>
         <v>-6.8000000000001393E-4</v>
       </c>
@@ -1323,27 +2025,27 @@
         <v>0</v>
       </c>
       <c r="L3">
-        <f t="shared" ref="K3:L3" si="0">D3-H3</f>
+        <f t="shared" ref="L3" si="0">D3-H3</f>
         <v>0.40000000000000036</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="12">
+      <c r="B4" s="18">
         <v>0.79608000000000012</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="19">
         <v>21.6</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="20">
         <v>5.4</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="12">
+      <c r="F4" s="6">
         <v>0.81188000000000005</v>
       </c>
       <c r="G4">
@@ -1352,7 +2054,7 @@
       <c r="H4">
         <v>4.8</v>
       </c>
-      <c r="J4" s="13">
+      <c r="J4" s="7">
         <f t="shared" ref="J4:J16" si="1">B4-F4</f>
         <v>-1.5799999999999925E-2</v>
       </c>
@@ -1366,22 +2068,22 @@
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="12">
+      <c r="B5" s="18">
         <v>0.7980600000000001</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="19">
         <v>10.8</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="20">
         <v>4</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="12">
+      <c r="F5" s="6">
         <v>0.75982000000000005</v>
       </c>
       <c r="G5">
@@ -1390,7 +2092,7 @@
       <c r="H5">
         <v>5.6</v>
       </c>
-      <c r="J5" s="13">
+      <c r="J5" s="7">
         <f t="shared" si="1"/>
         <v>3.8240000000000052E-2</v>
       </c>
@@ -1404,22 +2106,22 @@
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="12">
+      <c r="B6" s="18">
         <v>0.98074000000000017</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="19">
         <v>10.4</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="20">
         <v>0.6</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="F6" s="12">
+      <c r="F6" s="6">
         <v>0.99848000000000003</v>
       </c>
       <c r="G6">
@@ -1428,7 +2130,7 @@
       <c r="H6">
         <v>0.2</v>
       </c>
-      <c r="J6" s="13">
+      <c r="J6" s="7">
         <f t="shared" si="1"/>
         <v>-1.7739999999999867E-2</v>
       </c>
@@ -1442,22 +2144,22 @@
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="12">
+      <c r="B7" s="18">
         <v>0.97360000000000002</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="19">
         <v>13.2</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="20">
         <v>1.2</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="E7" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="F7" s="12">
+      <c r="F7" s="6">
         <v>0.97655999999999987</v>
       </c>
       <c r="G7">
@@ -1466,7 +2168,7 @@
       <c r="H7">
         <v>1.2</v>
       </c>
-      <c r="J7" s="13">
+      <c r="J7" s="7">
         <f t="shared" si="1"/>
         <v>-2.9599999999998516E-3</v>
       </c>
@@ -1480,22 +2182,22 @@
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="12">
+      <c r="B8" s="18">
         <v>0.84252000000000005</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="19">
         <v>21</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="20">
         <v>5.6</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="E8" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="F8" s="12">
+      <c r="F8" s="6">
         <v>0.82713999999999999</v>
       </c>
       <c r="G8">
@@ -1504,7 +2206,7 @@
       <c r="H8">
         <v>6.8</v>
       </c>
-      <c r="J8" s="13">
+      <c r="J8" s="7">
         <f t="shared" si="1"/>
         <v>1.538000000000006E-2</v>
       </c>
@@ -1518,22 +2220,22 @@
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="12">
+      <c r="B9" s="18">
         <v>0.87331999999999999</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="19">
         <v>11.4</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="20">
         <v>1.8</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="E9" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="F9" s="12">
+      <c r="F9" s="6">
         <v>0.89351999999999998</v>
       </c>
       <c r="G9">
@@ -1542,7 +2244,7 @@
       <c r="H9">
         <v>1.2</v>
       </c>
-      <c r="J9" s="13">
+      <c r="J9" s="7">
         <f t="shared" si="1"/>
         <v>-2.0199999999999996E-2</v>
       </c>
@@ -1556,22 +2258,22 @@
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="12">
+      <c r="B10" s="18">
         <v>0.96111999999999997</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="19">
         <v>15</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="20">
         <v>4.5999999999999996</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="E10" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="F10" s="12">
+      <c r="F10" s="6">
         <v>0.98007999999999984</v>
       </c>
       <c r="G10">
@@ -1580,7 +2282,7 @@
       <c r="H10">
         <v>4.4000000000000004</v>
       </c>
-      <c r="J10" s="13">
+      <c r="J10" s="7">
         <f t="shared" si="1"/>
         <v>-1.8959999999999866E-2</v>
       </c>
@@ -1594,22 +2296,22 @@
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="12">
+      <c r="B11" s="18">
         <v>0.96652000000000005</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="19">
         <v>10.8</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="20">
         <v>4.5999999999999996</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="E11" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="F11" s="12">
+      <c r="F11" s="6">
         <v>0.92160000000000009</v>
       </c>
       <c r="G11">
@@ -1618,7 +2320,7 @@
       <c r="H11">
         <v>5.4</v>
       </c>
-      <c r="J11" s="13">
+      <c r="J11" s="7">
         <f t="shared" si="1"/>
         <v>4.491999999999996E-2</v>
       </c>
@@ -1632,22 +2334,22 @@
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="12">
+      <c r="B12" s="18">
         <v>0.73433999999999999</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="19">
         <v>20.399999999999999</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="20">
         <v>8.8000000000000007</v>
       </c>
-      <c r="E12" s="10" t="s">
+      <c r="E12" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="F12" s="12">
+      <c r="F12" s="6">
         <v>0.7533200000000001</v>
       </c>
       <c r="G12">
@@ -1656,7 +2358,7 @@
       <c r="H12">
         <v>8.8000000000000007</v>
       </c>
-      <c r="J12" s="13">
+      <c r="J12" s="7">
         <f t="shared" si="1"/>
         <v>-1.8980000000000108E-2</v>
       </c>
@@ -1670,22 +2372,22 @@
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A13" s="10" t="s">
+      <c r="A13" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="12">
+      <c r="B13" s="18">
         <v>0.75403999999999993</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="19">
         <v>17.399999999999999</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="20">
         <v>6.4</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="E13" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="F13" s="12">
+      <c r="F13" s="6">
         <v>0.7585599999999999</v>
       </c>
       <c r="G13">
@@ -1694,7 +2396,7 @@
       <c r="H13">
         <v>5.8</v>
       </c>
-      <c r="J13" s="13">
+      <c r="J13" s="7">
         <f t="shared" si="1"/>
         <v>-4.5199999999999685E-3</v>
       </c>
@@ -1708,22 +2410,22 @@
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A14" s="10" t="s">
+      <c r="A14" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="12">
+      <c r="B14" s="18">
         <v>0.92145999999999995</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="19">
         <v>14.8</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="20">
         <v>2</v>
       </c>
-      <c r="E14" s="10" t="s">
+      <c r="E14" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="F14" s="12">
+      <c r="F14" s="6">
         <v>0.93423999999999996</v>
       </c>
       <c r="G14">
@@ -1732,7 +2434,7 @@
       <c r="H14">
         <v>1.8</v>
       </c>
-      <c r="J14" s="13">
+      <c r="J14" s="7">
         <f t="shared" si="1"/>
         <v>-1.2780000000000014E-2</v>
       </c>
@@ -1746,22 +2448,22 @@
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A15" s="10" t="s">
+      <c r="A15" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="12">
+      <c r="B15" s="18">
         <v>0.77636000000000005</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="19">
         <v>13.4</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="20">
         <v>3</v>
       </c>
-      <c r="E15" s="10" t="s">
+      <c r="E15" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="F15" s="12">
+      <c r="F15" s="6">
         <v>0.77338000000000007</v>
       </c>
       <c r="G15">
@@ -1770,7 +2472,7 @@
       <c r="H15">
         <v>3.4</v>
       </c>
-      <c r="J15" s="13">
+      <c r="J15" s="7">
         <f t="shared" si="1"/>
         <v>2.9799999999999827E-3</v>
       </c>
@@ -1784,22 +2486,22 @@
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A16" s="10" t="s">
+      <c r="A16" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="12">
+      <c r="B16" s="18">
         <v>0.97445999999999999</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="19">
         <v>18.2</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="20">
         <v>1</v>
       </c>
-      <c r="E16" s="10" t="s">
+      <c r="E16" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="F16" s="12">
+      <c r="F16" s="6">
         <v>0.97859999999999991</v>
       </c>
       <c r="G16">
@@ -1808,7 +2510,7 @@
       <c r="H16">
         <v>1.2</v>
       </c>
-      <c r="J16" s="13">
+      <c r="J16" s="7">
         <f t="shared" si="1"/>
         <v>-4.1399999999999215E-3</v>
       </c>
@@ -1821,12 +2523,619 @@
         <v>-0.19999999999999996</v>
       </c>
     </row>
+    <row r="19" spans="1:12" ht="26" x14ac:dyDescent="0.2">
+      <c r="A19" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19" s="14"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E20" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="J20" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="K20" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="L20" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" s="19">
+        <v>0.67977999999999994</v>
+      </c>
+      <c r="C21" s="19">
+        <v>5.4</v>
+      </c>
+      <c r="D21" s="20">
+        <v>7</v>
+      </c>
+      <c r="E21" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="F21" s="6">
+        <v>0.92495999999999989</v>
+      </c>
+      <c r="G21">
+        <v>13.8</v>
+      </c>
+      <c r="H21">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="J21" s="7">
+        <f>B21-F21</f>
+        <v>-0.24517999999999995</v>
+      </c>
+      <c r="K21">
+        <f>C21-G21</f>
+        <v>-8.4</v>
+      </c>
+      <c r="L21">
+        <f t="shared" ref="L21:L34" si="4">D21-H21</f>
+        <v>2.4000000000000004</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" s="19">
+        <v>0.47252</v>
+      </c>
+      <c r="C22" s="19">
+        <v>11.8</v>
+      </c>
+      <c r="D22" s="20">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="E22" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="F22" s="6">
+        <v>0.81188000000000005</v>
+      </c>
+      <c r="G22">
+        <v>22</v>
+      </c>
+      <c r="H22">
+        <v>4.8</v>
+      </c>
+      <c r="J22" s="7">
+        <f t="shared" ref="J22:J34" si="5">B22-F22</f>
+        <v>-0.33936000000000005</v>
+      </c>
+      <c r="K22">
+        <f t="shared" ref="K22:K34" si="6">C22-G22</f>
+        <v>-10.199999999999999</v>
+      </c>
+      <c r="L22">
+        <f t="shared" si="4"/>
+        <v>3.3999999999999995</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23" s="19">
+        <v>0.55556000000000005</v>
+      </c>
+      <c r="C23" s="19">
+        <v>5.2</v>
+      </c>
+      <c r="D23" s="20">
+        <v>2</v>
+      </c>
+      <c r="E23" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="F23" s="6">
+        <v>0.75982000000000005</v>
+      </c>
+      <c r="G23">
+        <v>10.6</v>
+      </c>
+      <c r="H23">
+        <v>5.6</v>
+      </c>
+      <c r="J23" s="7">
+        <f t="shared" si="5"/>
+        <v>-0.20426</v>
+      </c>
+      <c r="K23">
+        <f t="shared" si="6"/>
+        <v>-5.3999999999999995</v>
+      </c>
+      <c r="L23">
+        <f t="shared" si="4"/>
+        <v>-3.5999999999999996</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B24" s="19">
+        <v>0.85475999999999996</v>
+      </c>
+      <c r="C24" s="19">
+        <v>8.4</v>
+      </c>
+      <c r="D24" s="20">
+        <v>2.4</v>
+      </c>
+      <c r="E24" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="F24" s="6">
+        <v>0.99848000000000003</v>
+      </c>
+      <c r="G24">
+        <v>10.8</v>
+      </c>
+      <c r="H24">
+        <v>0.2</v>
+      </c>
+      <c r="J24" s="7">
+        <f t="shared" si="5"/>
+        <v>-0.14372000000000007</v>
+      </c>
+      <c r="K24">
+        <f t="shared" si="6"/>
+        <v>-2.4000000000000004</v>
+      </c>
+      <c r="L24">
+        <f t="shared" si="4"/>
+        <v>2.1999999999999997</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25" s="19">
+        <v>0.76783999999999997</v>
+      </c>
+      <c r="C25" s="19">
+        <v>10</v>
+      </c>
+      <c r="D25" s="20">
+        <v>5</v>
+      </c>
+      <c r="E25" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="F25" s="6">
+        <v>0.97655999999999987</v>
+      </c>
+      <c r="G25">
+        <v>13.2</v>
+      </c>
+      <c r="H25">
+        <v>1.2</v>
+      </c>
+      <c r="J25" s="7">
+        <f t="shared" si="5"/>
+        <v>-0.20871999999999991</v>
+      </c>
+      <c r="K25">
+        <f t="shared" si="6"/>
+        <v>-3.1999999999999993</v>
+      </c>
+      <c r="L25">
+        <f t="shared" si="4"/>
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26" s="19">
+        <v>0.55669999999999997</v>
+      </c>
+      <c r="C26" s="19">
+        <v>10.8</v>
+      </c>
+      <c r="D26" s="20">
+        <v>6.4</v>
+      </c>
+      <c r="E26" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="F26" s="6">
+        <v>0.82713999999999999</v>
+      </c>
+      <c r="G26">
+        <v>20.6</v>
+      </c>
+      <c r="H26">
+        <v>6.8</v>
+      </c>
+      <c r="J26" s="7">
+        <f t="shared" si="5"/>
+        <v>-0.27044000000000001</v>
+      </c>
+      <c r="K26">
+        <f t="shared" si="6"/>
+        <v>-9.8000000000000007</v>
+      </c>
+      <c r="L26">
+        <f t="shared" si="4"/>
+        <v>-0.39999999999999947</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B27" s="19">
+        <v>0.62538000000000005</v>
+      </c>
+      <c r="C27" s="19">
+        <v>7</v>
+      </c>
+      <c r="D27" s="20">
+        <v>1.2</v>
+      </c>
+      <c r="E27" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="F27" s="6">
+        <v>0.89351999999999998</v>
+      </c>
+      <c r="G27">
+        <v>11.6</v>
+      </c>
+      <c r="H27">
+        <v>1.2</v>
+      </c>
+      <c r="J27" s="7">
+        <f t="shared" si="5"/>
+        <v>-0.26813999999999993</v>
+      </c>
+      <c r="K27">
+        <f t="shared" si="6"/>
+        <v>-4.5999999999999996</v>
+      </c>
+      <c r="L27">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B28" s="19">
+        <v>0.88683999999999996</v>
+      </c>
+      <c r="C28" s="19">
+        <v>10.8</v>
+      </c>
+      <c r="D28" s="20">
+        <v>6</v>
+      </c>
+      <c r="E28" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="F28" s="6">
+        <v>0.98007999999999984</v>
+      </c>
+      <c r="G28">
+        <v>14.8</v>
+      </c>
+      <c r="H28">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="J28" s="7">
+        <f t="shared" si="5"/>
+        <v>-9.3239999999999879E-2</v>
+      </c>
+      <c r="K28">
+        <f t="shared" si="6"/>
+        <v>-4</v>
+      </c>
+      <c r="L28">
+        <f t="shared" si="4"/>
+        <v>1.5999999999999996</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B29" s="19">
+        <v>0.78746000000000005</v>
+      </c>
+      <c r="C29" s="19">
+        <v>7.6</v>
+      </c>
+      <c r="D29" s="20">
+        <v>4</v>
+      </c>
+      <c r="E29" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="F29" s="6">
+        <v>0.92160000000000009</v>
+      </c>
+      <c r="G29">
+        <v>10.8</v>
+      </c>
+      <c r="H29">
+        <v>5.4</v>
+      </c>
+      <c r="J29" s="7">
+        <f t="shared" si="5"/>
+        <v>-0.13414000000000004</v>
+      </c>
+      <c r="K29">
+        <f t="shared" si="6"/>
+        <v>-3.2000000000000011</v>
+      </c>
+      <c r="L29">
+        <f t="shared" si="4"/>
+        <v>-1.4000000000000004</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B30" s="19">
+        <v>0.48627999999999999</v>
+      </c>
+      <c r="C30" s="19">
+        <v>8</v>
+      </c>
+      <c r="D30" s="20">
+        <v>6.2</v>
+      </c>
+      <c r="E30" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="F30" s="6">
+        <v>0.7533200000000001</v>
+      </c>
+      <c r="G30">
+        <v>21.6</v>
+      </c>
+      <c r="H30">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="J30" s="7">
+        <f t="shared" si="5"/>
+        <v>-0.26704000000000011</v>
+      </c>
+      <c r="K30">
+        <f t="shared" si="6"/>
+        <v>-13.600000000000001</v>
+      </c>
+      <c r="L30">
+        <f t="shared" si="4"/>
+        <v>-2.6000000000000005</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B31" s="19">
+        <v>0.33400000000000002</v>
+      </c>
+      <c r="C31" s="19">
+        <v>2.6</v>
+      </c>
+      <c r="D31" s="20">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="E31" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="F31" s="6">
+        <v>0.7585599999999999</v>
+      </c>
+      <c r="G31">
+        <v>17.600000000000001</v>
+      </c>
+      <c r="H31">
+        <v>5.8</v>
+      </c>
+      <c r="J31" s="7">
+        <f t="shared" si="5"/>
+        <v>-0.42455999999999988</v>
+      </c>
+      <c r="K31">
+        <f t="shared" si="6"/>
+        <v>-15.000000000000002</v>
+      </c>
+      <c r="L31">
+        <f t="shared" si="4"/>
+        <v>-3.5999999999999996</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B32" s="19">
+        <v>0.53225999999999996</v>
+      </c>
+      <c r="C32" s="19">
+        <v>5.4</v>
+      </c>
+      <c r="D32" s="20">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="E32" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="F32" s="6">
+        <v>0.93423999999999996</v>
+      </c>
+      <c r="G32">
+        <v>14.6</v>
+      </c>
+      <c r="H32">
+        <v>1.8</v>
+      </c>
+      <c r="J32" s="7">
+        <f t="shared" si="5"/>
+        <v>-0.40198</v>
+      </c>
+      <c r="K32">
+        <f t="shared" si="6"/>
+        <v>-9.1999999999999993</v>
+      </c>
+      <c r="L32">
+        <f t="shared" si="4"/>
+        <v>2.8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B33" s="19">
+        <v>0.45218000000000008</v>
+      </c>
+      <c r="C33" s="19">
+        <v>6.6</v>
+      </c>
+      <c r="D33" s="20">
+        <v>3.4</v>
+      </c>
+      <c r="E33" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="F33" s="6">
+        <v>0.77338000000000007</v>
+      </c>
+      <c r="G33">
+        <v>13</v>
+      </c>
+      <c r="H33">
+        <v>3.4</v>
+      </c>
+      <c r="J33" s="7">
+        <f t="shared" si="5"/>
+        <v>-0.32119999999999999</v>
+      </c>
+      <c r="K33">
+        <f t="shared" si="6"/>
+        <v>-6.4</v>
+      </c>
+      <c r="L33">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B34" s="19">
+        <v>0.69170000000000009</v>
+      </c>
+      <c r="C34" s="19">
+        <v>11</v>
+      </c>
+      <c r="D34" s="20">
+        <v>5</v>
+      </c>
+      <c r="E34" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="F34" s="6">
+        <v>0.97859999999999991</v>
+      </c>
+      <c r="G34">
+        <v>18.2</v>
+      </c>
+      <c r="H34">
+        <v>1.2</v>
+      </c>
+      <c r="J34" s="7">
+        <f t="shared" si="5"/>
+        <v>-0.28689999999999982</v>
+      </c>
+      <c r="K34">
+        <f t="shared" si="6"/>
+        <v>-7.1999999999999993</v>
+      </c>
+      <c r="L34">
+        <f t="shared" si="4"/>
+        <v>3.8</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="E1:H1"/>
     <mergeCell ref="A1:D1"/>
+    <mergeCell ref="E19:H19"/>
+    <mergeCell ref="A19:D19"/>
   </mergeCells>
   <conditionalFormatting sqref="L3:L16">
+    <cfRule type="cellIs" dxfId="11" priority="7" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="8" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J3:K16">
+    <cfRule type="cellIs" dxfId="9" priority="5" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="6" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J21:K34">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L21:L34">
     <cfRule type="cellIs" dxfId="3" priority="3" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -1834,14 +3143,6 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J3:K16">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="86" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>